<commit_message>
#UPDATE: Architecture.xlsx and README.md.
</commit_message>
<xml_diff>
--- a/Architecture.xlsx
+++ b/Architecture.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="211" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="173" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -17,7 +17,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t>  The architecture of AndroidStringResourcesGenerator</t>
+    <t>The architecture of AndroidStringResourcesGenerator</t>
   </si>
 </sst>
 </file>
@@ -27,9 +27,10 @@
   <numFmts count="1">
     <numFmt formatCode="GENERAL" numFmtId="164"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="12">
     <font>
       <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <sz val="10"/>
     </font>
@@ -50,14 +51,8 @@
     </font>
     <font>
       <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
-      <sz val="12"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="2"/>
-      <b val="true"/>
-      <color rgb="FFFFFFFF"/>
       <sz val="12"/>
     </font>
     <font>
@@ -65,7 +60,7 @@
       <charset val="1"/>
       <family val="2"/>
       <b val="true"/>
-      <color rgb="FF000000"/>
+      <color rgb="FFFFFFFF"/>
       <sz val="12"/>
     </font>
     <font>
@@ -76,18 +71,34 @@
       <sz val="12"/>
     </font>
     <font>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <color rgb="FF000000"/>
+      <sz val="12"/>
+    </font>
+    <font>
       <name val="Arial"/>
-      <charset val="1"/>
       <family val="2"/>
       <b val="true"/>
       <sz val="12"/>
     </font>
     <font>
       <name val="Arial"/>
-      <charset val="1"/>
       <family val="2"/>
       <b val="true"/>
       <color rgb="FFDC2300"/>
+      <sz val="12"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="2"/>
+      <color rgb="FFDC2300"/>
+      <sz val="12"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="2"/>
+      <color rgb="FF000000"/>
       <sz val="12"/>
     </font>
   </fonts>
@@ -154,7 +165,7 @@
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="3" fontId="5" numFmtId="164" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="3" fontId="5" numFmtId="164" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -234,26 +245,114 @@
 <xdr:wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>250200</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>51120</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>198360</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>218160</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="0" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="759240" y="524520"/>
+          <a:ext cx="6823440" cy="1588320"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst>
+            <a:gd fmla="val 3600" name="adj"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="ffffff"/>
+        </a:solidFill>
+        <a:ln cap="rnd" w="36720">
+          <a:solidFill>
+            <a:srgbClr val="c5000b"/>
+          </a:solidFill>
+          <a:custDash>
+            <a:ds d="102000" sp="102000"/>
+          </a:custDash>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>247680</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>123480</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>196200</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>211680</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="756720" y="2491920"/>
+          <a:ext cx="6823800" cy="5535720"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst>
+            <a:gd fmla="val 3600" name="adj"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="ffffff"/>
+        </a:solidFill>
+        <a:ln cap="rnd" w="36720">
+          <a:solidFill>
+            <a:srgbClr val="c5000b"/>
+          </a:solidFill>
+          <a:custDash>
+            <a:ds d="102000" sp="102000"/>
+          </a:custDash>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>61200</xdr:colOff>
+      <xdr:colOff>115200</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>202680</xdr:rowOff>
+      <xdr:rowOff>184680</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>26</xdr:col>
-      <xdr:colOff>142920</xdr:colOff>
+      <xdr:colOff>196200</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>212040</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="0" name="Rectangle 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1334160" y="5650200"/>
-          <a:ext cx="5429160" cy="1904040"/>
+      <xdr:rowOff>193320</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1388160" y="5632200"/>
+          <a:ext cx="5428440" cy="1903320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -268,9 +367,13 @@
         </a:ln>
       </xdr:spPr>
       <xdr:txBody>
-        <a:bodyPr anchorCtr="1" bIns="91440" tIns="91440" wrap="none"/>
-        <a:p>
-          <a:pPr algn="ctr"/>
+        <a:bodyPr anchorCtr="1" bIns="91440" lIns="90000" rIns="90000" tIns="91440" wrap="none"/>
+        <a:p>
+          <a:pPr algn="ctr">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
           <a:r>
             <a:rPr b="1" lang="en-US">
               <a:solidFill>
@@ -283,7 +386,11 @@
           <a:endParaRPr/>
         </a:p>
         <a:p>
-          <a:pPr algn="just"/>
+          <a:pPr algn="just">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
           <a:r>
             <a:rPr b="1" lang="en-US">
               <a:solidFill>
@@ -302,25 +409,25 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>163080</xdr:colOff>
+      <xdr:colOff>217080</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>110160</xdr:rowOff>
+      <xdr:rowOff>92160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>193680</xdr:colOff>
+      <xdr:colOff>246960</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>61200</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="1" name="Rectangle 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1436040" y="6268320"/>
-          <a:ext cx="2067840" cy="1135080"/>
+      <xdr:rowOff>42480</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1490040" y="6250320"/>
+          <a:ext cx="2067120" cy="1134360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -335,9 +442,13 @@
         </a:ln>
       </xdr:spPr>
       <xdr:txBody>
-        <a:bodyPr anchorCtr="1" bIns="91440" tIns="91440" wrap="none"/>
-        <a:p>
-          <a:pPr algn="ctr"/>
+        <a:bodyPr anchorCtr="1" bIns="91440" lIns="90000" rIns="90000" tIns="91440" wrap="none"/>
+        <a:p>
+          <a:pPr algn="ctr">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
           <a:r>
             <a:rPr lang="en-US">
               <a:solidFill>
@@ -354,26 +465,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>213840</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>13320</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>60840</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>244800</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>11880</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="Rectangle 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4542480" y="6219000"/>
-          <a:ext cx="2067840" cy="1135080"/>
+      <xdr:rowOff>42840</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>43200</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>230040</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4596480" y="6201000"/>
+          <a:ext cx="2067120" cy="1134360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -388,9 +499,13 @@
         </a:ln>
       </xdr:spPr>
       <xdr:txBody>
-        <a:bodyPr anchorCtr="1" bIns="91440" tIns="91440" wrap="none"/>
-        <a:p>
-          <a:pPr algn="ctr"/>
+        <a:bodyPr anchorCtr="1" bIns="91440" lIns="90000" rIns="90000" tIns="91440" wrap="none"/>
+        <a:p>
+          <a:pPr algn="ctr">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
           <a:r>
             <a:rPr lang="en-US">
               <a:solidFill>
@@ -402,7 +517,11 @@
           <a:endParaRPr/>
         </a:p>
         <a:p>
-          <a:pPr algn="ctr"/>
+          <a:pPr algn="ctr">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
           <a:r>
             <a:rPr lang="en-US">
               <a:solidFill>
@@ -419,25 +538,25 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>239040</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>38520</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>179640</xdr:rowOff>
+      <xdr:rowOff>161640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>188280</xdr:colOff>
+      <xdr:colOff>242280</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>179640</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="Line 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3549240" y="6811560"/>
+      <xdr:rowOff>161640</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Line 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3603240" y="6793560"/>
           <a:ext cx="967680" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -457,25 +576,25 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>41400</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>14040</xdr:rowOff>
+      <xdr:colOff>95400</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>232920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>26</xdr:col>
-      <xdr:colOff>123120</xdr:colOff>
+      <xdr:colOff>176400</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>23400</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="Rectangle 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1314360" y="2856240"/>
-          <a:ext cx="5429160" cy="1904040"/>
+      <xdr:rowOff>4680</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1368360" y="2838240"/>
+          <a:ext cx="5428440" cy="1903320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -490,9 +609,13 @@
         </a:ln>
       </xdr:spPr>
       <xdr:txBody>
-        <a:bodyPr anchorCtr="1" bIns="91440" tIns="91440" wrap="none"/>
-        <a:p>
-          <a:pPr algn="ctr"/>
+        <a:bodyPr anchorCtr="1" bIns="91440" lIns="90000" rIns="90000" tIns="91440" wrap="none"/>
+        <a:p>
+          <a:pPr algn="ctr">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
           <a:r>
             <a:rPr b="1" lang="en-US">
               <a:solidFill>
@@ -505,7 +628,11 @@
           <a:endParaRPr/>
         </a:p>
         <a:p>
-          <a:pPr algn="ctr"/>
+          <a:pPr algn="ctr">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
           <a:r>
             <a:rPr b="1" lang="en-US">
               <a:solidFill>
@@ -518,7 +645,11 @@
           <a:endParaRPr/>
         </a:p>
         <a:p>
-          <a:pPr algn="ctr"/>
+          <a:pPr algn="ctr">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
           <a:r>
             <a:rPr b="1" lang="en-US">
               <a:solidFill>
@@ -526,25 +657,7 @@
               </a:solidFill>
               <a:latin typeface="Arial"/>
             </a:rPr>
-            <a:t>the </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="1" lang="en-US">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial"/>
-            </a:rPr>
-            <a:t>AndroidStringXML package's use</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="1" lang="en-US">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial"/>
-            </a:rPr>
-            <a:t>  </a:t>
+            <a:t>the AndroidStringXML package's use  </a:t>
           </a:r>
           <a:endParaRPr/>
         </a:p>
@@ -555,25 +668,25 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>153000</xdr:colOff>
+      <xdr:colOff>207000</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>159120</xdr:rowOff>
+      <xdr:rowOff>141120</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>183600</xdr:colOff>
+      <xdr:colOff>236880</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>110160</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="Rectangle 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1425960" y="3475080"/>
-          <a:ext cx="2067840" cy="1135080"/>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1479960" y="3457080"/>
+          <a:ext cx="2067120" cy="1134360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -588,9 +701,13 @@
         </a:ln>
       </xdr:spPr>
       <xdr:txBody>
-        <a:bodyPr anchorCtr="1" bIns="91440" tIns="91440" wrap="none"/>
-        <a:p>
-          <a:pPr algn="ctr"/>
+        <a:bodyPr anchorCtr="1" bIns="91440" lIns="90000" rIns="90000" tIns="91440" wrap="none"/>
+        <a:p>
+          <a:pPr algn="ctr">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
           <a:r>
             <a:rPr lang="en-US">
               <a:solidFill>
@@ -602,7 +719,11 @@
           <a:endParaRPr/>
         </a:p>
         <a:p>
-          <a:pPr algn="ctr"/>
+          <a:pPr algn="ctr">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
           <a:r>
             <a:rPr lang="en-US">
               <a:solidFill>
@@ -620,25 +741,25 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>193680</xdr:colOff>
+      <xdr:colOff>247680</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>165960</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>224640</xdr:colOff>
+      <xdr:rowOff>147960</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>23040</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>117000</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="Rectangle 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4522320" y="3481920"/>
-          <a:ext cx="2067840" cy="1135080"/>
+      <xdr:rowOff>98280</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4576320" y="3463920"/>
+          <a:ext cx="2067120" cy="1134360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -653,9 +774,13 @@
         </a:ln>
       </xdr:spPr>
       <xdr:txBody>
-        <a:bodyPr anchorCtr="1" bIns="91440" tIns="91440" wrap="none"/>
-        <a:p>
-          <a:pPr algn="ctr"/>
+        <a:bodyPr anchorCtr="1" bIns="91440" lIns="90000" rIns="90000" tIns="91440" wrap="none"/>
+        <a:p>
+          <a:pPr algn="ctr">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
           <a:r>
             <a:rPr lang="en-US">
               <a:solidFill>
@@ -667,7 +792,11 @@
           <a:endParaRPr/>
         </a:p>
         <a:p>
-          <a:pPr algn="ctr"/>
+          <a:pPr algn="ctr">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
           <a:r>
             <a:rPr lang="en-US">
               <a:solidFill>
@@ -679,7 +808,11 @@
           <a:endParaRPr/>
         </a:p>
         <a:p>
-          <a:pPr algn="ctr"/>
+          <a:pPr algn="ctr">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
           <a:r>
             <a:rPr lang="en-US">
               <a:solidFill>
@@ -691,7 +824,11 @@
           <a:endParaRPr/>
         </a:p>
         <a:p>
-          <a:pPr algn="ctr"/>
+          <a:pPr algn="ctr">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
           <a:r>
             <a:rPr lang="en-US">
               <a:solidFill>
@@ -703,7 +840,11 @@
           <a:endParaRPr/>
         </a:p>
         <a:p>
-          <a:pPr algn="ctr"/>
+          <a:pPr algn="ctr">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
           <a:r>
             <a:rPr lang="en-US">
               <a:solidFill>
@@ -720,25 +861,25 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>214200</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>13680</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>20880</xdr:rowOff>
+      <xdr:rowOff>2880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>163440</xdr:colOff>
+      <xdr:colOff>217440</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>20880</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="Line 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3524400" y="4047120"/>
+      <xdr:rowOff>2880</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="Line 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3578400" y="4029120"/>
           <a:ext cx="967680" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -758,25 +899,25 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>173160</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>12240</xdr:rowOff>
+      <xdr:colOff>227160</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>231120</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>81720</xdr:colOff>
+      <xdr:colOff>135000</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>71280</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="TextShape 1"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1955520" y="5222880"/>
-          <a:ext cx="1181520" cy="295920"/>
+      <xdr:rowOff>52560</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2009520" y="5204880"/>
+          <a:ext cx="1180800" cy="295200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -800,25 +941,25 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>132840</xdr:colOff>
+      <xdr:colOff>186840</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>158040</xdr:rowOff>
+      <xdr:rowOff>140040</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>163440</xdr:colOff>
+      <xdr:colOff>216720</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>108720</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name="Rectangle 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1405800" y="631440"/>
-          <a:ext cx="2067840" cy="1135080"/>
+      <xdr:rowOff>90000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1459800" y="613440"/>
+          <a:ext cx="2067120" cy="1134360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -833,9 +974,13 @@
         </a:ln>
       </xdr:spPr>
       <xdr:txBody>
-        <a:bodyPr anchorCtr="1" bIns="91440" tIns="91440" wrap="none"/>
-        <a:p>
-          <a:pPr algn="ctr"/>
+        <a:bodyPr anchorCtr="1" bIns="91440" lIns="90000" rIns="90000" tIns="91440" wrap="none"/>
+        <a:p>
+          <a:pPr algn="ctr">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
           <a:r>
             <a:rPr lang="en-US">
               <a:solidFill>
@@ -847,7 +992,11 @@
           <a:endParaRPr/>
         </a:p>
         <a:p>
-          <a:pPr algn="ctr"/>
+          <a:pPr algn="ctr">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
           <a:r>
             <a:rPr lang="en-US">
               <a:solidFill>
@@ -865,25 +1014,25 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>173520</xdr:colOff>
+      <xdr:colOff>227520</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>164880</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>204480</xdr:colOff>
+      <xdr:rowOff>146880</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>2880</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>115560</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="10" name="Rectangle 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4502160" y="638280"/>
-          <a:ext cx="2067840" cy="1135080"/>
+      <xdr:rowOff>96840</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4556160" y="620280"/>
+          <a:ext cx="2067120" cy="1134360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -898,9 +1047,13 @@
         </a:ln>
       </xdr:spPr>
       <xdr:txBody>
-        <a:bodyPr anchorCtr="1" bIns="91440" tIns="91440" wrap="none"/>
-        <a:p>
-          <a:pPr algn="ctr"/>
+        <a:bodyPr anchorCtr="1" bIns="91440" lIns="90000" rIns="90000" tIns="91440" wrap="none"/>
+        <a:p>
+          <a:pPr algn="ctr">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
           <a:r>
             <a:rPr lang="en-US">
               <a:solidFill>
@@ -912,7 +1065,11 @@
           <a:endParaRPr/>
         </a:p>
         <a:p>
-          <a:pPr algn="ctr"/>
+          <a:pPr algn="ctr">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
           <a:r>
             <a:rPr lang="en-US">
               <a:solidFill>
@@ -924,7 +1081,11 @@
           <a:endParaRPr/>
         </a:p>
         <a:p>
-          <a:pPr algn="ctr"/>
+          <a:pPr algn="ctr">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
           <a:r>
             <a:rPr lang="en-US">
               <a:solidFill>
@@ -936,7 +1097,11 @@
           <a:endParaRPr/>
         </a:p>
         <a:p>
-          <a:pPr algn="ctr"/>
+          <a:pPr algn="ctr">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
           <a:r>
             <a:rPr lang="en-US">
               <a:solidFill>
@@ -954,24 +1119,24 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>194040</xdr:colOff>
+      <xdr:colOff>248040</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>19440</xdr:rowOff>
+      <xdr:rowOff>1440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>143280</xdr:colOff>
+      <xdr:colOff>197280</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>19440</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="11" name="Line 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3504240" y="1203480"/>
+      <xdr:rowOff>1440</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="Line 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3558240" y="1185480"/>
           <a:ext cx="967680" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -990,70 +1155,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>193680</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>141480</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>29</xdr:col>
-      <xdr:colOff>142920</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>230400</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="12" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="702720" y="2509920"/>
-          <a:ext cx="6824520" cy="5536440"/>
-        </a:xfrm>
-        <a:prstGeom prst="roundRect">
-          <a:avLst>
-            <a:gd fmla="val 3600" name="adj"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="ffffff"/>
-        </a:solidFill>
-        <a:ln w="36720">
-          <a:solidFill>
-            <a:srgbClr val="c5000b"/>
-          </a:solidFill>
-          <a:custDash>
-            <a:ds d="197000" sp="197000"/>
-          </a:custDash>
-          <a:round/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="absolute">
-    <xdr:from>
-      <xdr:col>29</xdr:col>
-      <xdr:colOff>234360</xdr:colOff>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>33840</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>19800</xdr:rowOff>
+      <xdr:rowOff>1800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>40</xdr:col>
-      <xdr:colOff>183600</xdr:colOff>
+      <xdr:colOff>236880</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>123840</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="13" name="TextShape 1"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7618680" y="4993560"/>
-          <a:ext cx="2750040" cy="340920"/>
+      <xdr:rowOff>105120</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7672680" y="4975560"/>
+          <a:ext cx="2749320" cy="340200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1083,24 +1204,24 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>163080</xdr:colOff>
+      <xdr:colOff>217080</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>99000</xdr:rowOff>
+      <xdr:rowOff>81000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>163080</xdr:colOff>
+      <xdr:colOff>217080</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>138240</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="14" name="Line 1"/>
+      <xdr:rowOff>120240</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="Line 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="1945440" y="1756800"/>
+          <a:off x="1999440" y="1738800"/>
           <a:ext cx="0" cy="1697400"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1119,26 +1240,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>214200</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>13680</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>167760</xdr:rowOff>
+      <xdr:rowOff>149760</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>122760</xdr:colOff>
+      <xdr:colOff>176040</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>226800</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="15" name="TextShape 1"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1996560" y="1825560"/>
-          <a:ext cx="1181520" cy="295920"/>
+      <xdr:rowOff>208080</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2050560" y="1807560"/>
+          <a:ext cx="1180800" cy="295200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1162,24 +1283,24 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>91800</xdr:colOff>
+      <xdr:colOff>145800</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>119160</xdr:rowOff>
+      <xdr:rowOff>101160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>91800</xdr:colOff>
+      <xdr:colOff>145800</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>158400</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="16" name="Line 1"/>
+      <xdr:rowOff>140400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="17" name="Line 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="1874160" y="4619160"/>
+          <a:off x="1928160" y="4601160"/>
           <a:ext cx="0" cy="1697400"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1199,25 +1320,25 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>720</xdr:colOff>
+      <xdr:colOff>54720</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>76680</xdr:rowOff>
+      <xdr:rowOff>58680</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>26</xdr:col>
-      <xdr:colOff>82440</xdr:colOff>
+      <xdr:colOff>135720</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>105840</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="17" name="Rectangle 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1273680" y="9077040"/>
-          <a:ext cx="5429160" cy="1213560"/>
+      <xdr:rowOff>87120</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1327680" y="9059040"/>
+          <a:ext cx="5428440" cy="1212840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1232,7 +1353,7 @@
         </a:ln>
       </xdr:spPr>
       <xdr:txBody>
-        <a:bodyPr anchor="ctr" bIns="91440" tIns="164520" wrap="none"/>
+        <a:bodyPr anchor="ctr" bIns="91440" lIns="90000" rIns="90000" tIns="164520" wrap="none"/>
         <a:p>
           <a:r>
             <a:rPr b="1" lang="en-US">
@@ -1315,24 +1436,24 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>51480</xdr:colOff>
+      <xdr:colOff>105480</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>50040</xdr:rowOff>
+      <xdr:rowOff>32040</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>51480</xdr:colOff>
+      <xdr:colOff>105480</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>89280</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="18" name="Line 1"/>
+      <xdr:rowOff>71280</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="19" name="Line 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="1833840" y="7392240"/>
+          <a:off x="1887840" y="7374240"/>
           <a:ext cx="0" cy="1697400"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1352,25 +1473,25 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>98280</xdr:colOff>
+      <xdr:colOff>152280</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>99360</xdr:rowOff>
+      <xdr:rowOff>81360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>6840</xdr:colOff>
+      <xdr:colOff>60120</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>158400</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="19" name="TextShape 1"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1880640" y="7678440"/>
-          <a:ext cx="1181520" cy="295920"/>
+      <xdr:rowOff>139680</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="20" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1934640" y="7660440"/>
+          <a:ext cx="1180800" cy="295200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1393,70 +1514,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>196200</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>69120</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>29</xdr:col>
-      <xdr:colOff>145080</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>236880</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="20" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="705240" y="542520"/>
-          <a:ext cx="6824160" cy="1589040"/>
-        </a:xfrm>
-        <a:prstGeom prst="roundRect">
-          <a:avLst>
-            <a:gd fmla="val 3600" name="adj"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="ffffff"/>
-        </a:solidFill>
-        <a:ln w="36720">
-          <a:solidFill>
-            <a:srgbClr val="c5000b"/>
-          </a:solidFill>
-          <a:custDash>
-            <a:ds d="197000" sp="197000"/>
-          </a:custDash>
-          <a:round/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="absolute">
-    <xdr:from>
-      <xdr:col>29</xdr:col>
-      <xdr:colOff>234720</xdr:colOff>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>34200</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>187920</xdr:rowOff>
+      <xdr:rowOff>169920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>40</xdr:col>
-      <xdr:colOff>183960</xdr:colOff>
+      <xdr:colOff>237240</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>225360</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="21" name="TextShape 1"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7619040" y="898200"/>
-          <a:ext cx="2750040" cy="511200"/>
+      <xdr:rowOff>206640</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="21" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7673040" y="880200"/>
+          <a:ext cx="2749320" cy="510480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1472,7 +1549,19 @@
               </a:solidFill>
               <a:latin typeface="Arial"/>
             </a:rPr>
-            <a:t>The source of string resources, should be implemented by case.</a:t>
+            <a:t>The source of string resources, </a:t>
+          </a:r>
+          <a:endParaRPr/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr b="1" lang="en-US">
+              <a:solidFill>
+                <a:srgbClr val="dc2300"/>
+              </a:solidFill>
+              <a:latin typeface="Arial"/>
+            </a:rPr>
+            <a:t>should be implemented by case.</a:t>
           </a:r>
           <a:endParaRPr/>
         </a:p>
@@ -1494,7 +1583,7 @@
   <dimension ref="B2:S65536"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="AG37" activeCellId="0" pane="topLeft" sqref="AG37"/>
+      <selection activeCell="AN18" activeCellId="0" pane="topLeft" sqref="AN18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.65"/>

</xml_diff>